<commit_message>
unit 61 - intermediate
</commit_message>
<xml_diff>
--- a/homework/61.xlsx
+++ b/homework/61.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22624"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6C7DBE5-045A-45AB-A5CB-2FED4B1C59F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E19E46D-83E7-4374-84AA-B0F5DECFC1DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9180" yWindow="4560" windowWidth="19470" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6495" yWindow="2190" windowWidth="19470" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,97 +23,134 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
-  <si>
-    <t>61.2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>61.3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>61.4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">used to </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>got used to</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>wasn't used to working</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>is used to working</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>got(get) used to</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>is used to (driving)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>am used to sleeping on the floor</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>am used to working long hours</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>I'm not used to going to bed (so) late</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>get used to living</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>get used to driving two hours to work</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>get(got) used to (the) new teacher</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>drink</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>eating</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>having</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>go</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>live,living</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>is(being)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>build(be)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>drive(have)</t>
+    <t>62.2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>62.3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>doing</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>coming</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>buying</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>seeing</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>solving</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>playing(watching)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>going(spending/having)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>of causing</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>from walking</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>for interrupting</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>of using</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>from escaping</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>on telling</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>to eating</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>for being</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>for inviting</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>of,wearing</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>of</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/about</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> doing</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>on taking to the station</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>on getting married</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>to me for not phoning earlier</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>me of (being) selfish</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>me(Sue) for coming to see her</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -121,7 +158,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -137,6 +174,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
@@ -525,8 +571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:C58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -541,189 +587,218 @@
   <sheetData>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" s="1">
-        <v>61.1</v>
+        <v>62.1</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B4" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B5" s="1">
+        <v>3</v>
+      </c>
       <c r="C5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B6" s="1">
+        <v>4</v>
+      </c>
       <c r="C6" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B7" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="C8" s="6" t="s">
+      <c r="B8" s="1">
+        <v>6</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B9" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="C9" s="1" t="s">
-        <v>6</v>
+      <c r="C9" s="6" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="B10" s="5"/>
+      <c r="B10" s="5">
+        <v>8</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A11" s="2" t="s">
+      <c r="B11" s="5">
+        <v>9</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="5"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="B12" s="5">
-        <v>2</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="B12" s="5"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="B13" s="5">
-        <v>3</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="A13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="5"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B14" s="5">
+        <v>2</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B15" s="5">
+        <v>3</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B16" s="5">
         <v>4</v>
       </c>
-      <c r="C14" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="B15" s="5"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A16" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16" s="5"/>
+      <c r="C16" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B17" s="5">
-        <v>2</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>14</v>
+        <v>5</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B18" s="5">
-        <v>3</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B19" s="5">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="B20" s="5"/>
+      <c r="B20" s="5">
+        <v>8</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A21" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B21" s="5"/>
+      <c r="B21" s="5">
+        <v>9</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B22" s="5">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B23" s="5">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B24" s="5">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="B25" s="5">
-        <v>5</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>22</v>
-      </c>
+      <c r="B25" s="5"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="B26" s="5">
-        <v>6</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="A26" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" s="5"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B27" s="5">
-        <v>7</v>
-      </c>
-      <c r="C27" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B28" s="5">
-        <v>8</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>20</v>
+        <v>3</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B29" s="5">
-        <v>9</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>19</v>
+        <v>4</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="B30" s="5"/>
+      <c r="B30" s="5">
+        <v>5</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="B31" s="5"/>
+      <c r="B31" s="5">
+        <v>6</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B32" s="5"/>

</xml_diff>

<commit_message>
unit 63 - intermediate
</commit_message>
<xml_diff>
--- a/homework/61.xlsx
+++ b/homework/61.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22624"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E19E46D-83E7-4374-84AA-B0F5DECFC1DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6C7DBE5-045A-45AB-A5CB-2FED4B1C59F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6495" yWindow="2190" windowWidth="19470" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9180" yWindow="4560" windowWidth="19470" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,134 +23,97 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+  <si>
+    <t>61.2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>61.3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>61.4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">used to </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>got used to</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wasn't used to working</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>is used to working</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>got(get) used to</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>is used to (driving)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>am used to sleeping on the floor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>am used to working long hours</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I'm not used to going to bed (so) late</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>get used to living</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>get used to driving two hours to work</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>get(got) used to (the) new teacher</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>drink</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>eating</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
   <si>
     <t>having</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>62.2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>62.3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>doing</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>coming</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>buying</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>seeing</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>solving</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>playing(watching)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>going(spending/having)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>of causing</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>from walking</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>for interrupting</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>of using</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>from escaping</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>on telling</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>to eating</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>for being</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>for inviting</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>of,wearing</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>of</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>/about</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> doing</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>on taking to the station</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>on getting married</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>to me for not phoning earlier</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>me of (being) selfish</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>me(Sue) for coming to see her</t>
+    <t>go</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>live,living</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>is(being)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>build(be)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>drive(have)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -158,7 +121,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -174,15 +137,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <strike/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
@@ -571,8 +525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:C58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -587,218 +541,189 @@
   <sheetData>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" s="1">
-        <v>62.1</v>
+        <v>61.1</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B4" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="B5" s="1">
-        <v>3</v>
-      </c>
       <c r="C5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="B6" s="1">
-        <v>4</v>
-      </c>
       <c r="C6" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B7" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="B8" s="1">
+      <c r="C8" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="B9" s="1">
-        <v>7</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="B10" s="5">
-        <v>8</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="B10" s="5"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="B11" s="5">
+      <c r="A11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="5"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B12" s="5">
+        <v>2</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="B12" s="5"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A13" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B13" s="5"/>
+      <c r="B13" s="5">
+        <v>3</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B14" s="5">
-        <v>2</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="B15" s="5">
-        <v>3</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="B15" s="5"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="B16" s="5">
-        <v>4</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="A16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="5"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B17" s="5">
-        <v>5</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>13</v>
+        <v>2</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B18" s="5">
-        <v>6</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>20</v>
+        <v>3</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B19" s="5">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="B20" s="5">
-        <v>8</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="B20" s="5"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="B21" s="5">
-        <v>9</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="A21" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" s="5"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B22" s="5">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B23" s="5">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B24" s="5">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="B25" s="5"/>
+      <c r="B25" s="5">
+        <v>5</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A26" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B26" s="5"/>
+      <c r="B26" s="5">
+        <v>6</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B27" s="5">
-        <v>2</v>
-      </c>
-      <c r="C27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="6" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B28" s="5">
-        <v>3</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>22</v>
+        <v>8</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B29" s="5">
-        <v>4</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>25</v>
+        <v>9</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="B30" s="5">
-        <v>5</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>23</v>
-      </c>
+      <c r="B30" s="5"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="B31" s="5">
-        <v>6</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>24</v>
-      </c>
+      <c r="B31" s="5"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B32" s="5"/>

</xml_diff>